<commit_message>
moved I2C interrupt pin to pin 33 (previous pin was not able to set the pullup)
</commit_message>
<xml_diff>
--- a/electronic design/esp pin mapping.xlsx
+++ b/electronic design/esp pin mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e733add8f175125d/Documenten/Pim Swinkels Creative Engineering/Opdrachten/Fiction Factory/Dior - kinetic Wall/Dior - kinetic wall Engineering/electronic design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="8_{13F88AF0-670C-4E6F-BCA2-3C40FE81AF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{675CBE8D-1DA0-451E-AC91-94F0368B07DC}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="8_{13F88AF0-670C-4E6F-BCA2-3C40FE81AF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C775ACE-9DBB-4DBE-A369-4D1E0C6C9828}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="11235" windowWidth="29040" windowHeight="15720" xr2:uid="{62D6CD04-D730-40FE-9ECB-DE266D67FC03}"/>
   </bookViews>
@@ -642,7 +642,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1025,6 +1025,9 @@
       <c r="B29" t="s">
         <v>7</v>
       </c>
+      <c r="F29" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
@@ -1038,9 +1041,6 @@
       </c>
       <c r="D30" t="s">
         <v>13</v>
-      </c>
-      <c r="F30" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
6 row installation working. functional for the interactive installation
</commit_message>
<xml_diff>
--- a/electronic design/esp pin mapping.xlsx
+++ b/electronic design/esp pin mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e733add8f175125d/Documenten/Pim Swinkels Creative Engineering/Opdrachten/Fiction Factory/Dior - kinetic Wall/Dior - kinetic wall Engineering/electronic design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="8_{13F88AF0-670C-4E6F-BCA2-3C40FE81AF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C775ACE-9DBB-4DBE-A369-4D1E0C6C9828}"/>
+  <xr:revisionPtr revIDLastSave="233" documentId="8_{13F88AF0-670C-4E6F-BCA2-3C40FE81AF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08C26F50-33C7-4913-900A-81CEAC585FFF}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="11235" windowWidth="29040" windowHeight="15720" xr2:uid="{62D6CD04-D730-40FE-9ECB-DE266D67FC03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62D6CD04-D730-40FE-9ECB-DE266D67FC03}"/>
   </bookViews>
   <sheets>
     <sheet name="interactive_installation_V1" sheetId="1" r:id="rId1"/>
@@ -641,19 +641,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA74ADF2-825A-47A8-99E8-3FCFAA462051}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -676,7 +676,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -690,7 +690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -704,7 +704,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -718,7 +718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -732,7 +732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -743,7 +743,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -754,7 +754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -765,7 +765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -776,7 +776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -787,7 +787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -798,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -809,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -820,7 +820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -840,7 +840,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -854,7 +854,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -868,7 +868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -882,7 +882,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -890,10 +890,10 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -901,10 +901,10 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -915,7 +915,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -926,7 +926,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -943,7 +943,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -960,7 +960,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -971,7 +971,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -985,7 +985,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
@@ -999,7 +999,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>32</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>33</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>34</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>35</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>36</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>39</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>32</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>35</v>
       </c>

</xml_diff>